<commit_message>
Atualizacao historico de vagas
</commit_message>
<xml_diff>
--- a/vagas.xlsx
+++ b/vagas.xlsx
@@ -10,7 +10,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet1'!$A$1:$N$1153</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet1'!$A$1:$Q$1153</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -451,7 +451,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N1153"/>
+  <dimension ref="A1:Q1153"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -535,6 +535,21 @@
           <t>Nova Adição</t>
         </is>
       </c>
+      <c r="O1" s="2" t="inlineStr">
+        <is>
+          <t>Unnamed: 14</t>
+        </is>
+      </c>
+      <c r="P1" s="2" t="inlineStr">
+        <is>
+          <t>Unnamed: 15</t>
+        </is>
+      </c>
+      <c r="Q1" s="2" t="inlineStr">
+        <is>
+          <t>Unnamed: 16</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -591,13 +606,14 @@
           <t>hybrid</t>
         </is>
       </c>
-      <c r="M2">
-        <f>HYPERLINK("https://visagio.gupy.io/job/eyJqb2JJZCI6ODk5NTk5Miwic291cmNlIjoiZ3VweV9wb3J0YWwifQ==?jobBoardSource=gupy_portal", "https://visagio.gupy.io/job/eyJqb2JJZCI6ODk5NTk5Miwic291cmNlIjoiZ3VweV9wb3J0YWwifQ==?jobBoardSource=gupy_portal")</f>
-        <v/>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>https://visagio.gupy.io/job/eyJqb2JJZCI6ODk5NTk5Miwic291cmNlIjoiZ3VweV9wb3J0YWwifQ==?jobBoardSource=gupy_portal</t>
+        </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
     </row>
@@ -1467,6 +1483,12 @@
           <t>Não</t>
         </is>
       </c>
+      <c r="P16" t="n">
+        <v>35</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>0.06060606060606055</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="3" t="n">
@@ -1583,6 +1605,9 @@
           <t>Não</t>
         </is>
       </c>
+      <c r="P18" t="n">
+        <v>33</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="3" t="n">
@@ -71395,7 +71420,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N1153"/>
+  <autoFilter ref="A1:Q1153"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>